<commit_message>
Fix LED problem and update Pins
Builtin LED not working for some reason, so add external LED which works. Update this in Pins to reflect the new hardware. Text deciphering still not working
</commit_message>
<xml_diff>
--- a/Arduino/Pins.xlsx
+++ b/Arduino/Pins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\Arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhay\Documents\ArduinoRockets\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E02D28F-6D31-4561-B383-12E3427D6F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A25CB5C-C96D-409C-8DEC-6C93395C7F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Accessory</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>MOSI = COPI, MISO = CIPO, CS = SS</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>longer, +</t>
+  </si>
+  <si>
+    <t>shorter, -</t>
+  </si>
+  <si>
+    <t>D5</t>
   </si>
 </sst>
 </file>
@@ -240,14 +252,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -566,25 +578,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" style="2" customWidth="1"/>
-    <col min="3" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="14.3984375" style="2" customWidth="1"/>
+    <col min="3" max="10" width="9.1328125" style="2"/>
+    <col min="11" max="11" width="10.73046875" style="2" customWidth="1"/>
     <col min="12" max="12" width="11" style="2" customWidth="1"/>
-    <col min="13" max="18" width="9.140625" style="2"/>
-    <col min="19" max="19" width="10.5703125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="2"/>
-    <col min="21" max="21" width="10.7109375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="2"/>
+    <col min="13" max="18" width="9.1328125" style="2"/>
+    <col min="19" max="19" width="10.59765625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.1328125" style="2"/>
+    <col min="21" max="21" width="10.73046875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="11.59765625" style="2" customWidth="1"/>
+    <col min="23" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -604,8 +616,8 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -639,9 +651,13 @@
         <v>33</v>
       </c>
       <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="X2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A3" s="7"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -705,9 +721,15 @@
       <c r="W3" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="X3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -774,15 +796,21 @@
       <c r="W4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="X4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -808,43 +836,43 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -853,7 +881,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -862,7 +890,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -870,7 +898,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -878,7 +906,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -886,7 +914,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -894,7 +922,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -902,7 +930,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -910,7 +938,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -918,11 +946,11 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.45">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C36" s="6" t="s">
         <v>6</v>
       </c>
@@ -934,11 +962,11 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="8" t="s">
+    <row r="37" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C37" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="9"/>
       <c r="F37" s="5"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -961,128 +989,136 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+    <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
       <c r="E38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="7"/>
-      <c r="V38" s="7"/>
-      <c r="W38" s="7"/>
-      <c r="X38" s="7"/>
-      <c r="Y38" s="7"/>
-      <c r="Z38" s="7"/>
-    </row>
-    <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+    </row>
+    <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="7"/>
-      <c r="V39" s="7"/>
-      <c r="W39" s="7"/>
-      <c r="X39" s="7"/>
-      <c r="Y39" s="7"/>
-      <c r="Z39" s="7"/>
-    </row>
-    <row r="40" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+    </row>
+    <row r="40" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="7"/>
-      <c r="V40" s="7"/>
-      <c r="W40" s="7"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
-      <c r="Z40" s="7"/>
-    </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+    </row>
+    <row r="41" spans="3:26" x14ac:dyDescent="0.45">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="7"/>
-      <c r="V41" s="7"/>
-      <c r="W41" s="7"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="7"/>
-      <c r="Z41" s="7"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F38:Z38"/>
+    <mergeCell ref="F39:Z39"/>
+    <mergeCell ref="F40:Z40"/>
+    <mergeCell ref="F41:Z41"/>
+    <mergeCell ref="C37:D41"/>
+    <mergeCell ref="E36:H36"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="A2:A6"/>
@@ -1090,13 +1126,6 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F38:Z38"/>
-    <mergeCell ref="F39:Z39"/>
-    <mergeCell ref="F40:Z40"/>
-    <mergeCell ref="F41:Z41"/>
-    <mergeCell ref="C37:D41"/>
-    <mergeCell ref="E36:H36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F38" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>

</xml_diff>

<commit_message>
Reformatted the Pins file
</commit_message>
<xml_diff>
--- a/Arduino/Pins.xlsx
+++ b/Arduino/Pins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\src\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C01D5B-33E0-45B0-88AD-5113288B3E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693458B7-D799-434F-B6A4-D142CEC23E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
@@ -252,14 +252,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -576,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
-  <dimension ref="A1:Z41"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +617,7 @@
       <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -657,7 +657,7 @@
       <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="7"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -729,7 +729,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -804,13 +804,13 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -847,270 +847,194 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="3:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="8" t="s">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-    </row>
-    <row r="38" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="2" t="s">
+      <c r="D17" s="9"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="7"/>
-      <c r="V38" s="7"/>
-      <c r="W38" s="7"/>
-      <c r="X38" s="7"/>
-      <c r="Y38" s="7"/>
-      <c r="Z38" s="7"/>
-    </row>
-    <row r="39" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="2" t="s">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="7"/>
-      <c r="V39" s="7"/>
-      <c r="W39" s="7"/>
-      <c r="X39" s="7"/>
-      <c r="Y39" s="7"/>
-      <c r="Z39" s="7"/>
-    </row>
-    <row r="40" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="2" t="s">
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="7"/>
-      <c r="V40" s="7"/>
-      <c r="W40" s="7"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
-      <c r="Z40" s="7"/>
-    </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="2" t="s">
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="7"/>
-      <c r="V41" s="7"/>
-      <c r="W41" s="7"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="7"/>
-      <c r="Z41" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F18:Z18"/>
+    <mergeCell ref="F19:Z19"/>
+    <mergeCell ref="F20:Z20"/>
+    <mergeCell ref="F21:Z21"/>
+    <mergeCell ref="C17:D21"/>
+    <mergeCell ref="E16:H16"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
@@ -1119,19 +1043,12 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F38:Z38"/>
-    <mergeCell ref="F39:Z39"/>
-    <mergeCell ref="F40:Z40"/>
-    <mergeCell ref="F41:Z41"/>
-    <mergeCell ref="C37:D41"/>
-    <mergeCell ref="E36:H36"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F38" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
-    <hyperlink ref="F39" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
-    <hyperlink ref="F40" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
-    <hyperlink ref="F41" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>
+    <hyperlink ref="F18" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>
+    <hyperlink ref="F19" r:id="rId2" xr:uid="{5050C1D4-A2B3-49B0-A31A-26368B5FB3AE}"/>
+    <hyperlink ref="F20" r:id="rId3" xr:uid="{22D30853-0A8C-4606-A419-D79377A024AE}"/>
+    <hyperlink ref="F21" r:id="rId4" xr:uid="{71C3A2A6-029A-49E1-8624-C845751B4B71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Added NRF pins to Arduino UNO using the linked datasheet
</commit_message>
<xml_diff>
--- a/Arduino/Pins.xlsx
+++ b/Arduino/Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\src\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693458B7-D799-434F-B6A4-D142CEC23E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0E4535-1271-4086-B058-93FFADD3D234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-53805" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>Accessory</t>
   </si>
@@ -154,15 +154,6 @@
     <t>3V3</t>
   </si>
   <si>
-    <t>52 - SCK</t>
-  </si>
-  <si>
-    <t>50 - MISO</t>
-  </si>
-  <si>
-    <t>51 - MOSI</t>
-  </si>
-  <si>
     <t>https://howtomechatronics.com/tutorials/arduino/arduino-wireless-communication-nrf24l01-tutorial/</t>
   </si>
   <si>
@@ -188,6 +179,27 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D51 - MOSI</t>
+  </si>
+  <si>
+    <t>D52 - SCK</t>
+  </si>
+  <si>
+    <t>D50 - MISO</t>
   </si>
 </sst>
 </file>
@@ -252,14 +264,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -576,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +608,7 @@
     <col min="23" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -616,8 +628,8 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -652,12 +664,17 @@
       </c>
       <c r="W2" s="6"/>
       <c r="X2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Y2" s="6"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="Z2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -722,14 +739,23 @@
         <v>24</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Y3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -797,20 +823,50 @@
         <v>9</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="O5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -827,25 +883,25 @@
         <v>32</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -854,7 +910,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -863,27 +919,27 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="8"/>
       <c r="F17" s="5"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -907,134 +963,128 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
+      <c r="F18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
     </row>
     <row r="19" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
+      <c r="F19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
     </row>
     <row r="20" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
+      <c r="F20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
       <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
+      <c r="F21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F18:Z18"/>
-    <mergeCell ref="F19:Z19"/>
-    <mergeCell ref="F20:Z20"/>
-    <mergeCell ref="F21:Z21"/>
-    <mergeCell ref="C17:D21"/>
-    <mergeCell ref="E16:H16"/>
+  <mergeCells count="16">
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="C1:R1"/>
@@ -1043,6 +1093,13 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F18:Z18"/>
+    <mergeCell ref="F19:Z19"/>
+    <mergeCell ref="F20:Z20"/>
+    <mergeCell ref="F21:Z21"/>
+    <mergeCell ref="C17:D21"/>
+    <mergeCell ref="E16:H16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F18" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>

</xml_diff>

<commit_message>
Fixed bugs in RemoteLaunchReceiver and had a successful test
</commit_message>
<xml_diff>
--- a/Arduino/Pins.xlsx
+++ b/Arduino/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Rockets\Electronics\src\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0E4535-1271-4086-B058-93FFADD3D234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C197A3EC-1C07-4804-866F-BFE7E7DBE5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53805" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
+    <workbookView xWindow="-22230" yWindow="705" windowWidth="21600" windowHeight="11385" xr2:uid="{9F0E2A1F-6841-4F27-9638-8F05D0997AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,14 +264,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1DC071-A6C6-4B47-94A4-DDBFF84D3BAA}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
       <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -674,7 +674,7 @@
       <c r="AB2" s="6"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="7"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -755,7 +755,7 @@
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -830,7 +830,7 @@
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -866,7 +866,7 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -936,10 +936,10 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="3:26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="9"/>
       <c r="F17" s="5"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -963,127 +963,134 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="3:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F18:Z18"/>
+    <mergeCell ref="F19:Z19"/>
+    <mergeCell ref="F20:Z20"/>
+    <mergeCell ref="F21:Z21"/>
+    <mergeCell ref="C17:D21"/>
+    <mergeCell ref="E16:H16"/>
     <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="V2:W2"/>
@@ -1093,13 +1100,6 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="O2:U2"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F18:Z18"/>
-    <mergeCell ref="F19:Z19"/>
-    <mergeCell ref="F20:Z20"/>
-    <mergeCell ref="F21:Z21"/>
-    <mergeCell ref="C17:D21"/>
-    <mergeCell ref="E16:H16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F18" r:id="rId1" xr:uid="{AF6F9FDB-463C-42B8-B0DE-9750FB0836BF}"/>

</xml_diff>